<commit_message>
add new exercises, update anki deck/wordlist, description
- updated description for problem B in lesson 6 listening comprehension to improve clarity. (#133)
- updated anki deck/wordlist for Lesson 16. (3rd ed.)
- added the following exercises.

# Lesson 16 (3rd ed.)
- Kanji Vocabulary: 供, 世, 界, and 全
- Kanji Vocabulary: 部, 始, and 週
- Kanji Vocabulary: 考, 開, and 屋
- Kanji Vocabulary: 方, 運, and 動
- Kanji Vocabulary: 教, 室, and 以
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-16.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-16.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1057,6 +1057,834 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>child</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>子供|こども</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>to offer something to a spirit</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>供える|そなえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>offer</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>提供|ていきょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>the world</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>世界|せかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>care</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>世話|せわ</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>generation</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>世代|せだい</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>the third generation</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>三世|さんせい</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>society</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>世の中|よのなか</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>visibility</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>視界|しかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>political world</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>政界|せいかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>limit</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>限界|げんかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>all; entire</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>全部|ぜんぶ</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>safety</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>安全|あんぜん</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>whole country</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>全国|ぜんこく</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>entirely</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>全く|まったく</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>everything; all</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>全て|すべて</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>all; entire</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>全部|ぜんぶ</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>room</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>部屋|へや</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>tennis club</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>テニス部|テニスぶ</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>department manager</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>部長|ぶちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>(something) begins</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>始まる|はじまる</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>to begin (something)</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>始める|はじめる</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>first train (of the day)</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>始発|しはつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>開始|かいし</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>every week</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>毎週|まいしゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>last week</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>先週|せんしゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>one week</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>一週間|いっしゅうかん</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>second week</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>二週目|にしゅうめ</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>weekend</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>週末|しゅうまつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>to think</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>考える|かんがえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>idea</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>考え|かんがえ</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>archeology</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>考古学|こうこがく</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>参考|さんこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>to open (something)</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>開ける|あける</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>(something) opens</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>開く|あく</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>to open</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>開く|ひらく</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>opening of a store</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>開店|かいてん</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>room</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>部屋|へや</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>bookstore</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>本屋|ほんや</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>fish shop</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>魚屋|さかなや</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>rooftop</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>屋上|おくじょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>indoor</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>屋内|おくない</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>ally; person on one's side</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>味方|みかた</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>way of reading</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>読み方|よみかた</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>evening</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>夕方|ゆうがた</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>both</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>両方|りょうほう</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>方法|ほうほう</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>exercise</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>運動|うんどう</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>driving</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>運転|うんてん</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>lucky</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>運がいい|うんがいい</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>fate</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>運命|うんめい</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>to carry</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>運ぶ|はこぶ</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>to move</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>動く|うごく</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>automobile</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>自動車|じどうしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>animal</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>動物|どうぶつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>verb</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>動詞|どうし</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>to teach</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>教える|おしえる</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>教室|きょうしつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>church</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>教会|きょうかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Christianity</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>キリスト教|キリストきょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>textbook</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>教科書|きょうかしょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>professor's office</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>研究室|けんきゅうしつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>basement</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>地下室|ちかしつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>waiting room</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>待合室|まちあいしつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>other than...</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>～以外|～いがい</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>...or more</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>～以上|～いじょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>...or less</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>～以下|～いか</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>within...</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>～以内|～いない</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>before; formerly</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>以前|いぜん</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>